<commit_message>
update the list of vulnerabilities
</commit_message>
<xml_diff>
--- a/docs/list_defined_vulnerability.xlsx
+++ b/docs/list_defined_vulnerability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viet Anh Phan\Desktop\Trash documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6380F283-2F67-40F5-A07F-A101294D43F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC46A334-F109-4F23-B592-4A777B708D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="5025" windowWidth="28800" windowHeight="15885" xr2:uid="{EA03AD05-F9FA-4160-9777-1A1CF52484FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{EA03AD05-F9FA-4160-9777-1A1CF52484FB}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -282,6 +282,18 @@
   </si>
   <si>
     <t>Device only responds to illegitimate MLDv1 queries even though MLDv2 queries are sent, possibly downgraded</t>
+  </si>
+  <si>
+    <t>PTV-NET-MITM-ICMP6REDIR</t>
+  </si>
+  <si>
+    <t>PTV-NET-MITM-ICMP6REDIRDEV</t>
+  </si>
+  <si>
+    <t>Network does not block ICMPv6 Redirect messages</t>
+  </si>
+  <si>
+    <t>Device communication can be redirected using ICMPv6 Redirect</t>
   </si>
 </sst>
 </file>
@@ -656,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1230AB-46B8-4FDC-B377-3F44751E20F1}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,6 +1200,34 @@
         <v>65</v>
       </c>
     </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>